<commit_message>
read in problem/target file
</commit_message>
<xml_diff>
--- a/app/static/example_data/embrace-plus_problemtarget_large.xlsx
+++ b/app/static/example_data/embrace-plus_problemtarget_large.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fivoornl-my.sharepoint.com/personal/p_de_looff_fivoor_nl/Documents/Shares/Veerle_Hypebright/Wearables comparison/Veerle_28-3-2024_EmbracePlus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veerlevanleemput/Documents/Hypebright BV/Fivoor/wearalyze/app/static/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D7E72E75-0E8F-4E9F-9A51-EB3E70568734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B436898-2CA1-4145-BD6B-2E3C309012B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36885" yWindow="2940" windowWidth="21600" windowHeight="11235" xr2:uid="{530518F5-DA1D-40F8-A271-153060523471}"/>
+    <workbookView xWindow="36880" yWindow="2940" windowWidth="21600" windowHeight="11240" xr2:uid="{530518F5-DA1D-40F8-A271-153060523471}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -38,9 +37,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>Day</t>
-  </si>
-  <si>
     <t>Problem or Target Behavior</t>
   </si>
   <si>
@@ -48,6 +44,9 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -88,7 +87,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -422,76 +421,74 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0820842F-8F5E-44F1-9F8C-5AC83A240FD4}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>44931</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>44932</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>44933</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>44934</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>44935</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>2</v>

</xml_diff>

<commit_message>
update problem target files
</commit_message>
<xml_diff>
--- a/app/static/example_data/embrace-plus_problemtarget_large.xlsx
+++ b/app/static/example_data/embrace-plus_problemtarget_large.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veerlevanleemput/Documents/Hypebright BV/Fivoor/wearalyze/app/static/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B436898-2CA1-4145-BD6B-2E3C309012B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{980CB5F4-492C-5042-8792-3F97931C5A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36880" yWindow="2940" windowWidth="21600" windowHeight="11240" xr2:uid="{530518F5-DA1D-40F8-A271-153060523471}"/>
+    <workbookView xWindow="18960" yWindow="2640" windowWidth="24860" windowHeight="18360" xr2:uid="{530518F5-DA1D-40F8-A271-153060523471}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -35,12 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
   <si>
     <t>Problem or Target Behavior</t>
-  </si>
-  <si>
-    <t>Depression</t>
   </si>
   <si>
     <t>Score</t>
@@ -48,13 +45,24 @@
   <si>
     <t>Date</t>
   </si>
+  <si>
+    <t>Stress</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -82,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,79 +428,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0820842F-8F5E-44F1-9F8C-5AC83A240FD4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>44931</v>
+        <v>45434</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>44932</v>
+        <v>45435</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>44933</v>
+        <v>45436</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>44934</v>
+        <v>45437</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>44935</v>
+        <v>45438</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45439</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45440</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45441</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>